<commit_message>
revise data format, implement testing framework using JDoodle queries
</commit_message>
<xml_diff>
--- a/Backend/test_db.xlsx
+++ b/Backend/test_db.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Year4\From Idea to App\Final Project\DeveloCoop\Backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB344C3-94DA-48C7-BA71-C372789679C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -236,46 +242,6 @@
 			if S[i] != S[len(S) - i - 1]:
 				return 0
 		return 1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def gcd_answer(a, b):
-		"""
-		type a: int
-		type b: int
-		type return: int
-		"""
-		# base case: if b is 0, return a as gcd.
-		if b == 0:
-			return a
-		# recursively calling gcd function with b and a % b.
-		return self.gcd(b, a % b)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Function to perform binary search recursively
-	def bin_search(arr, left, right, k):
-		if left &gt; right:
-			return -1  # If left pointer exceeds right pointer, element not found
-		mid = (left + right) // 2  # Calculate mid index
-		if arr[mid] == k:
-			return mid  # If element is found at mid index, return index
-		if arr[mid] &gt; k:
-			return self.bin_search(
-				arr, left, mid - 1, k
-			)  # If element is less than mid, perform binary search on left subarray
-		else:
-			return self.bin_search(
-				arr, mid + 1, right, k
-			)  # If element is greater than mid, perform binary search on right subarray
-	def binarysearch_answer(arr, k):
-		"""
-		type k: int
-		type arr: List[int]
-		type return: int
-		"""
-		n = len(arr)
-		return self.bin_search(arr, 0, n - 1, k)  # Perform binary search on the entire array
 </t>
   </si>
   <si>
@@ -379,27 +345,67 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">def gcd_answer(a, b):
+		"""
+		type a: int
+		type b: int
+		type return: int
+		"""
+		# base case: if b is 0, return a as gcd.
+		if b == 0:
+			return a
+		# recursively calling gcd function with b and a % b.
+		return gcd_answer(b, a % b)
+</t>
+  </si>
+  <si>
     <t>test_cases = [
-	([1, 2, 3, 4, 5], 3),
-	([10, 20, 30, 40, 50], 25),
-	([7, 14, 21, 28, 35], 35),
-	([1, 1, 1, 1, 1], 1),
-	([2, 4, 6, 8, 10], 11),
-	([5, 10, 15, 20, 25, 30], 15),
-	([0, 2, 4, 6, 8, 10], 0),
-	([100, 200, 300, 400], 150),
-	([3, 6, 9, 12, 15, 18], 9),
-	([1, 3, 5, 7, 9], 8)
+    ([100, 180, 260, 310, 40, 535, 695], 7),
+    ([100, 180, 260, 310, 40, 535, 695, 200, 300, 250], 10),
+    ([7, 1, 5, 3, 6, 4], 6),
+    ([1, 2, 3, 4, 5], 5),
+    ([7, 6, 4, 3, 1], 5),
+    ([100, 90, 80, 70, 60, 50, 40], 7),
+    ([1, 2, 1, 2, 1, 2, 1, 2], 8),
+    ([10, 20, 30, 40, 50, 60, 70, 80], 8),
+    ([80, 70, 60, 50, 40, 30, 20, 10], 8),
+    ([100, 200, 300, 400, 500, 600, 700, 800, 900, 1000], 10)
 ]
 user_solution = stockBuySell
 solution = stockBuySell_answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Function to perform binary search recursively
+def bin_search(arr, left, right, k):
+    if left &gt; right:
+        return -1  # If left pointer exceeds right pointer, element not found
+    mid = (left + right) // 2  # Calculate mid index
+    if arr[mid] == k:
+        return mid  # If element is found at mid index, return index
+    if arr[mid] &gt; k:
+        return bin_search(
+            arr, left, mid - 1, k
+        )  # If element is less than mid, perform binary search on left subarray
+    else:
+        return bin_search(
+            arr, mid + 1, right, k
+        )  # If element is greater than mid, perform binary search on right subarray
+def binarysearch_answer(arr, k):
+    """
+    type k: int
+    type arr: List[int]
+    type return: int
+    """
+    n = len(arr)
+    return bin_search(arr, 0, n - 1, k)  # Perform binary search on the entire arrayy
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,10 +457,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,13 +471,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -506,7 +523,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -540,6 +557,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -574,9 +592,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,14 +768,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,41 +799,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -817,14 +843,14 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -834,14 +860,14 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -852,10 +878,10 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main db creation WIP
</commit_message>
<xml_diff>
--- a/Backend/test_db.xlsx
+++ b/Backend/test_db.xlsx
@@ -1,23 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Year4\From Idea to App\Final Project\DeveloCoop\Backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB344C3-94DA-48C7-BA71-C372789679C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
@@ -771,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -812,7 +792,7 @@
       <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>